<commit_message>
Added SeleniumJava_ExitTest Project Update
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-project-workspace\SeleniumJava_ExitTest\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9258100B-C728-4113-96DA-8828537BE499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E0A6B9-AD50-4585-B6E1-BCE4F8044266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="3045" windowWidth="11760" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>passwprd</t>
+    <t>password</t>
   </si>
   <si>
-    <t>user@gmail.con</t>
+    <t>ntwano14@gmail.com</t>
+  </si>
+  <si>
+    <t>NTWAno@16</t>
   </si>
 </sst>
 </file>
@@ -362,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,13 +388,17 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>12345</v>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{A9F624D3-CC59-47DD-B012-59565C749C47}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{E7833E4A-F84C-47B0-A61B-32E21D7DC2D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>